<commit_message>
add time estimation files
</commit_message>
<xml_diff>
--- a/time_estimation/time_estimation.xlsx
+++ b/time_estimation/time_estimation.xlsx
@@ -1,73 +1,98 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d18ab4ce63646fc5/Documenten/TU Delft/Thesis/Code/time_estimation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="11_F25DC773A252ABDACC10480D819E61165ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A176F32-7546-42B3-9D45-4D652E4BD633}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_2BB1D69C5B2056D2439D38524D3088B35299F65D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{389ED47B-B11E-476C-AF2C-4EC65F1AEEE9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="780" windowWidth="21600" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Filename</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>File name</t>
+  </si>
+  <si>
+    <t>Volume [mm3]</t>
+  </si>
+  <si>
+    <t>Area [mm2]</t>
+  </si>
+  <si>
+    <t>Height [mm]</t>
+  </si>
+  <si>
+    <t>Height^2 [mm2]</t>
+  </si>
+  <si>
+    <t>Height^3 [mm3]</t>
+  </si>
+  <si>
+    <t>Beam_100x30mm.stl</t>
+  </si>
+  <si>
+    <t>Beam_30x100mm.stl</t>
+  </si>
+  <si>
+    <t>Cube_50mm.stl</t>
+  </si>
+  <si>
+    <t>Cylinder_10x50mm.stl</t>
+  </si>
+  <si>
+    <t>Cylinder_50x50mm.stl</t>
+  </si>
+  <si>
+    <t>Plate_10mm.stl</t>
+  </si>
+  <si>
+    <t>Pyramid_40mm.stl</t>
   </si>
   <si>
     <t>Time [s]</t>
-  </si>
-  <si>
-    <t>Area [mm2]</t>
-  </si>
-  <si>
-    <t>Volume [mm3]</t>
-  </si>
-  <si>
-    <t>Height [mm]</t>
-  </si>
-  <si>
-    <t>Support Volume [mm3]</t>
-  </si>
-  <si>
-    <t>Cube</t>
-  </si>
-  <si>
-    <t>Sphere</t>
-  </si>
-  <si>
-    <t>Cilinder</t>
-  </si>
-  <si>
-    <t>Plate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,7 +103,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -86,18 +111,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -120,44 +163,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -184,15 +227,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -219,7 +261,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -231,263 +272,374 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
+        <v>90000</v>
+      </c>
+      <c r="C2">
+        <v>13800</v>
+      </c>
+      <c r="D2">
         <v>100</v>
       </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>25</v>
-      </c>
       <c r="E2">
-        <v>10</v>
+        <v>10000</v>
       </c>
       <c r="F2">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1000000</v>
+      </c>
+      <c r="G2">
+        <f>(120+30)*60</f>
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3">
-        <v>21</v>
+        <v>90000</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>13800</v>
       </c>
       <c r="D3">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E3">
-        <v>114</v>
+        <v>900</v>
       </c>
       <c r="F3">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27000</v>
+      </c>
+      <c r="G3">
+        <f>(60+55)*60</f>
+        <v>6900</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4">
-        <v>544</v>
+        <v>125000</v>
       </c>
       <c r="C4">
-        <v>24</v>
+        <v>15000</v>
       </c>
       <c r="D4">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E4">
-        <v>13</v>
+        <v>2500</v>
       </c>
       <c r="F4">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>125000</v>
+      </c>
+      <c r="G4">
+        <f>(2*60+24)*60</f>
+        <v>8640</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5">
-        <v>569</v>
+        <v>3924.3010299656939</v>
       </c>
       <c r="C5">
-        <v>61</v>
+        <v>1727.4993534451301</v>
       </c>
       <c r="D5">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="E5">
-        <v>15</v>
+        <v>2500</v>
       </c>
       <c r="F5">
-        <v>18</v>
+        <v>125000</v>
+      </c>
+      <c r="G5">
+        <f>29*60</f>
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>98152.154952251323</v>
+      </c>
+      <c r="C6">
+        <v>11779.615498434559</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+      <c r="E6">
+        <v>2500</v>
+      </c>
+      <c r="F6">
+        <v>125000</v>
+      </c>
+      <c r="G6">
+        <f>(60+51)*60</f>
+        <v>6660</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>399999.99999999988</v>
+      </c>
+      <c r="C7">
+        <v>88000</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>1000</v>
+      </c>
+      <c r="G7">
+        <f>(8*60+26)*60</f>
+        <v>30360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>18475.209554036319</v>
+      </c>
+      <c r="C8">
+        <v>4800.0001221054636</v>
+      </c>
+      <c r="D8">
+        <v>34.641017913818359</v>
+      </c>
+      <c r="E8">
+        <v>1200.000122105484</v>
+      </c>
+      <c r="F8">
+        <v>41569.225726440309</v>
+      </c>
+      <c r="G8">
+        <f>43*60</f>
+        <v>2580</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update extract_characteristics, slicing and extraction combined
</commit_message>
<xml_diff>
--- a/time_estimation/time_estimation.xlsx
+++ b/time_estimation/time_estimation.xlsx
@@ -1,103 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d18ab4ce63646fc5/Documenten/TU Delft/Thesis/Code/time_estimation/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_2BB1D69C5B2056D2439D38524D3088B35299F65D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{389ED47B-B11E-476C-AF2C-4EC65F1AEEE9}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="780" windowWidth="21600" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>File name</t>
-  </si>
-  <si>
-    <t>Volume [mm3]</t>
-  </si>
-  <si>
-    <t>Area [mm2]</t>
-  </si>
-  <si>
-    <t>Height [mm]</t>
-  </si>
-  <si>
-    <t>Height^2 [mm2]</t>
-  </si>
-  <si>
-    <t>Height^3 [mm3]</t>
-  </si>
-  <si>
-    <t>Beam_100x30mm.stl</t>
-  </si>
-  <si>
-    <t>Beam_30x100mm.stl</t>
-  </si>
-  <si>
-    <t>Cube_50mm.stl</t>
-  </si>
-  <si>
-    <t>Cylinder_10x50mm.stl</t>
-  </si>
-  <si>
-    <t>Cylinder_50x50mm.stl</t>
-  </si>
-  <si>
-    <t>Plate_10mm.stl</t>
-  </si>
-  <si>
-    <t>Pyramid_40mm.stl</t>
-  </si>
-  <si>
-    <t>Time [s]</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -112,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -436,207 +420,229 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>File name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Volume [mm3]</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Area [mm2]</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Height [mm]</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Height^2 [mm2]</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Height^3 [mm3]</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Time [s]</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Beam_100x30mm</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>90000</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>13800</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>100</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>10000</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="n">
         <v>1000000</v>
       </c>
-      <c r="G2">
-        <f>(120+30)*60</f>
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
+      <c r="G2" t="n">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Beam_30x100mm</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>90000</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>13800</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>30</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>900</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="n">
         <v>27000</v>
       </c>
-      <c r="G3">
-        <f>(60+55)*60</f>
-        <v>6900</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
+      <c r="G3" t="n">
+        <v>6817</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Cube_50mm</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>125000</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>15000</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>50</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="n">
         <v>2500</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="n">
         <v>125000</v>
       </c>
-      <c r="G4">
-        <f>(2*60+24)*60</f>
-        <v>8640</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>3924.3010299656939</v>
-      </c>
-      <c r="C5">
-        <v>1727.4993534451301</v>
-      </c>
-      <c r="D5">
+      <c r="G4" t="n">
+        <v>8616</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cylinder_10x50mm</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3924.301029965694</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1727.49935344513</v>
+      </c>
+      <c r="D5" t="n">
         <v>50</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="n">
         <v>2500</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="n">
         <v>125000</v>
       </c>
-      <c r="G5">
-        <f>29*60</f>
-        <v>1740</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="G5" t="n">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cylinder_50x50mm</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>98152.15495225132</v>
+      </c>
+      <c r="C6" t="n">
+        <v>11779.61549843456</v>
+      </c>
+      <c r="D6" t="n">
+        <v>50</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2500</v>
+      </c>
+      <c r="F6" t="n">
+        <v>125000</v>
+      </c>
+      <c r="G6" t="n">
+        <v>6638</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Plate_10mm</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>399999.9999999999</v>
+      </c>
+      <c r="C7" t="n">
+        <v>88000</v>
+      </c>
+      <c r="D7" t="n">
         <v>10</v>
       </c>
-      <c r="B6">
-        <v>98152.154952251323</v>
-      </c>
-      <c r="C6">
-        <v>11779.615498434559</v>
-      </c>
-      <c r="D6">
-        <v>50</v>
-      </c>
-      <c r="E6">
-        <v>2500</v>
-      </c>
-      <c r="F6">
-        <v>125000</v>
-      </c>
-      <c r="G6">
-        <f>(60+51)*60</f>
-        <v>6660</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>399999.99999999988</v>
-      </c>
-      <c r="C7">
-        <v>88000</v>
-      </c>
-      <c r="D7">
-        <v>10</v>
-      </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>100</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="n">
         <v>1000</v>
       </c>
-      <c r="G7">
-        <f>(8*60+26)*60</f>
-        <v>30360</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>18475.209554036319</v>
-      </c>
-      <c r="C8">
-        <v>4800.0001221054636</v>
-      </c>
-      <c r="D8">
-        <v>34.641017913818359</v>
-      </c>
-      <c r="E8">
+      <c r="G7" t="n">
+        <v>30346</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Pyramid_40mm</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>18475.20955403632</v>
+      </c>
+      <c r="C8" t="n">
+        <v>4800.000122105464</v>
+      </c>
+      <c r="D8" t="n">
+        <v>34.64101791381836</v>
+      </c>
+      <c r="E8" t="n">
         <v>1200.000122105484</v>
       </c>
-      <c r="F8">
-        <v>41569.225726440309</v>
-      </c>
-      <c r="G8">
-        <f>43*60</f>
-        <v>2580</v>
+      <c r="F8" t="n">
+        <v>41569.22572644031</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2578</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move extract_characteristics script to main statement
</commit_message>
<xml_diff>
--- a/time_estimation/time_estimation.xlsx
+++ b/time_estimation/time_estimation.xlsx
@@ -1,37 +1,90 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d18ab4ce63646fc5/Documenten/TU Delft/Thesis/Code/time_estimation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_2BB1D69C5B2057D090CB4932433088B35299F555" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0F217B7-D425-4736-B001-795B4FC7D978}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView minimized="1" xWindow="5080" yWindow="1950" windowWidth="28800" windowHeight="15290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>File name</t>
+  </si>
+  <si>
+    <t>Volume [mm3]</t>
+  </si>
+  <si>
+    <t>Area [mm2]</t>
+  </si>
+  <si>
+    <t>Height [mm]</t>
+  </si>
+  <si>
+    <t>Height^2 [mm2]</t>
+  </si>
+  <si>
+    <t>Height^3 [mm3]</t>
+  </si>
+  <si>
+    <t>Time [s]</t>
+  </si>
+  <si>
+    <t>Beam_100x30mm</t>
+  </si>
+  <si>
+    <t>Beam_30x100mm</t>
+  </si>
+  <si>
+    <t>Cube_50mm</t>
+  </si>
+  <si>
+    <t>Cylinder_10x50mm</t>
+  </si>
+  <si>
+    <t>Cylinder_50x50mm</t>
+  </si>
+  <si>
+    <t>Plate_10mm</t>
+  </si>
+  <si>
+    <t>Pyramid_40mm</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +99,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,228 +423,197 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>File name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Volume [mm3]</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Area [mm2]</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Height [mm]</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Height^2 [mm2]</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Height^3 [mm3]</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Time [s]</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Beam_100x30mm</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
         <v>90000</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>13800</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>100</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>10000</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>1000000</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>8999</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Beam_30x100mm</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
         <v>90000</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>13800</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>30</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>900</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>27000</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>6817</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Cube_50mm</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
         <v>125000</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>15000</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>50</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>2500</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>125000</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>8616</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Cylinder_10x50mm</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>3924.301029965694</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1727.49935344513</v>
-      </c>
-      <c r="D5" t="n">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>3924.3010299656939</v>
+      </c>
+      <c r="C5">
+        <v>1727.4993534451301</v>
+      </c>
+      <c r="D5">
         <v>50</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>2500</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>125000</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>1720</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Cylinder_50x50mm</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>98152.15495225132</v>
-      </c>
-      <c r="C6" t="n">
-        <v>11779.61549843456</v>
-      </c>
-      <c r="D6" t="n">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>98152.154952251323</v>
+      </c>
+      <c r="C6">
+        <v>11779.615498434559</v>
+      </c>
+      <c r="D6">
         <v>50</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>2500</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>125000</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>6638</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Plate_10mm</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>399999.9999999999</v>
-      </c>
-      <c r="C7" t="n">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>399999.99999999988</v>
+      </c>
+      <c r="C7">
         <v>88000</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>10</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>100</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>1000</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>30346</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Pyramid_40mm</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>18475.20955403632</v>
-      </c>
-      <c r="C8" t="n">
-        <v>4800.000122105464</v>
-      </c>
-      <c r="D8" t="n">
-        <v>34.64101791381836</v>
-      </c>
-      <c r="E8" t="n">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>18475.209554036319</v>
+      </c>
+      <c r="C8">
+        <v>4800.0001221054636</v>
+      </c>
+      <c r="D8">
+        <v>34.641017913818359</v>
+      </c>
+      <c r="E8">
         <v>1200.000122105484</v>
       </c>
-      <c r="F8" t="n">
-        <v>41569.22572644031</v>
-      </c>
-      <c r="G8" t="n">
+      <c r="F8">
+        <v>41569.225726440309</v>
+      </c>
+      <c r="G8">
         <v>2578</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update time estimation, add latex figures
</commit_message>
<xml_diff>
--- a/time_estimation/time_estimation.xlsx
+++ b/time_estimation/time_estimation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d18ab4ce63646fc5/Documenten/TU Delft/Thesis/Code/time_estimation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2BB1D69C5B2057D090CB4932433088B35299F555" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0F217B7-D425-4736-B001-795B4FC7D978}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_15C1348A5B00D05637F83111595ED87656CD9F4A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD522825-34A1-4FA9-B15F-D2D6CDE0B13F}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5080" yWindow="1950" windowWidth="28800" windowHeight="15290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="28800" windowHeight="15290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>File name</t>
   </si>
@@ -34,12 +34,6 @@
     <t>Height [mm]</t>
   </si>
   <si>
-    <t>Height^2 [mm2]</t>
-  </si>
-  <si>
-    <t>Height^3 [mm3]</t>
-  </si>
-  <si>
     <t>Time [s]</t>
   </si>
   <si>
@@ -62,6 +56,96 @@
   </si>
   <si>
     <t>Pyramid_40mm</t>
+  </si>
+  <si>
+    <t>3D_Printer_test_fixed_stl_3rd_gen</t>
+  </si>
+  <si>
+    <t>acoustic_plat</t>
+  </si>
+  <si>
+    <t>Another_dremel_bit_holder</t>
+  </si>
+  <si>
+    <t>bathroom_paper_roll_holder_with_shelf</t>
+  </si>
+  <si>
+    <t>Cap</t>
+  </si>
+  <si>
+    <t>Cute_axolotl_v5</t>
+  </si>
+  <si>
+    <t>Cylinder</t>
+  </si>
+  <si>
+    <t>Dancing_Happy_Dragon</t>
+  </si>
+  <si>
+    <t>Dewalt_Drill_Holder</t>
+  </si>
+  <si>
+    <t>ragon_statu</t>
+  </si>
+  <si>
+    <t>Flexi-Rex-improv</t>
+  </si>
+  <si>
+    <t>Flexy_PLA</t>
+  </si>
+  <si>
+    <t>full_flexi_possuml</t>
+  </si>
+  <si>
+    <t>FU_COIN_FINAL_12_31</t>
+  </si>
+  <si>
+    <t>HairTieBobbyPinBox</t>
+  </si>
+  <si>
+    <t>Low_poly_otter_3</t>
+  </si>
+  <si>
+    <t>Modern_Geometric_Planter</t>
+  </si>
+  <si>
+    <t>name_plat</t>
+  </si>
+  <si>
+    <t>Octopus_with_top_hat_for_some_reason</t>
+  </si>
+  <si>
+    <t>PCIE_Display_Stand4</t>
+  </si>
+  <si>
+    <t>Philips_OneBlade_Razor_Station</t>
+  </si>
+  <si>
+    <t>RubberDuck</t>
+  </si>
+  <si>
+    <t>scrapper_v5</t>
+  </si>
+  <si>
+    <t>Shark_popcorn_bowl</t>
+  </si>
+  <si>
+    <t>SM_Buddha_print</t>
+  </si>
+  <si>
+    <t>Speed_Squar</t>
+  </si>
+  <si>
+    <t>Swan</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>VaseV846</t>
+  </si>
+  <si>
+    <t>case</t>
   </si>
 </sst>
 </file>
@@ -137,6 +221,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -424,16 +512,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,16 +536,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>7</v>
       </c>
       <c r="B2">
         <v>90000</v>
@@ -470,18 +551,12 @@
         <v>100</v>
       </c>
       <c r="E2">
-        <v>10000</v>
-      </c>
-      <c r="F2">
-        <v>1000000</v>
-      </c>
-      <c r="G2">
         <v>8999</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>90000</v>
@@ -493,18 +568,12 @@
         <v>30</v>
       </c>
       <c r="E3">
-        <v>900</v>
-      </c>
-      <c r="F3">
-        <v>27000</v>
-      </c>
-      <c r="G3">
         <v>6817</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>125000</v>
@@ -516,18 +585,12 @@
         <v>50</v>
       </c>
       <c r="E4">
-        <v>2500</v>
-      </c>
-      <c r="F4">
-        <v>125000</v>
-      </c>
-      <c r="G4">
         <v>8616</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>3924.3010299656939</v>
@@ -539,18 +602,12 @@
         <v>50</v>
       </c>
       <c r="E5">
-        <v>2500</v>
-      </c>
-      <c r="F5">
-        <v>125000</v>
-      </c>
-      <c r="G5">
         <v>1720</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>98152.154952251323</v>
@@ -562,18 +619,12 @@
         <v>50</v>
       </c>
       <c r="E6">
-        <v>2500</v>
-      </c>
-      <c r="F6">
-        <v>125000</v>
-      </c>
-      <c r="G6">
         <v>6638</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>399999.99999999988</v>
@@ -585,18 +636,12 @@
         <v>10</v>
       </c>
       <c r="E7">
-        <v>100</v>
-      </c>
-      <c r="F7">
-        <v>1000</v>
-      </c>
-      <c r="G7">
         <v>30346</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>18475.209554036319</v>
@@ -608,13 +653,517 @@
         <v>34.641017913818359</v>
       </c>
       <c r="E8">
-        <v>1200.000122105484</v>
-      </c>
-      <c r="F8">
-        <v>41569.225726440309</v>
-      </c>
-      <c r="G8">
         <v>2578</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>48701.611744031121</v>
+      </c>
+      <c r="C9">
+        <v>42737.72194506447</v>
+      </c>
+      <c r="D9">
+        <v>60.522235870361328</v>
+      </c>
+      <c r="E9">
+        <v>16440</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>313750.00000000017</v>
+      </c>
+      <c r="C10">
+        <v>74000</v>
+      </c>
+      <c r="D10">
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <v>26275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>143591.84771055059</v>
+      </c>
+      <c r="C11">
+        <v>50565.076410959482</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>23167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>632926.45120755211</v>
+      </c>
+      <c r="C12">
+        <v>103166.7185681635</v>
+      </c>
+      <c r="D12">
+        <v>185.93342590332031</v>
+      </c>
+      <c r="E12">
+        <v>59451</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>5378.5681143174716</v>
+      </c>
+      <c r="C13">
+        <v>2548.046221391171</v>
+      </c>
+      <c r="D13">
+        <v>12.50000035762787</v>
+      </c>
+      <c r="E13">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14">
+        <v>12756.302435755561</v>
+      </c>
+      <c r="C14">
+        <v>14777.15722902477</v>
+      </c>
+      <c r="D14">
+        <v>21.79999923706055</v>
+      </c>
+      <c r="E14">
+        <v>4743</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>545347.3514940599</v>
+      </c>
+      <c r="C15">
+        <v>64131.482762952903</v>
+      </c>
+      <c r="D15">
+        <v>76.063808441162109</v>
+      </c>
+      <c r="E15">
+        <v>29663</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>10004.086661324771</v>
+      </c>
+      <c r="C16">
+        <v>10260.452771781769</v>
+      </c>
+      <c r="D16">
+        <v>56.5</v>
+      </c>
+      <c r="E16">
+        <v>4778</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>11907.500194774781</v>
+      </c>
+      <c r="C17">
+        <v>8387.9595668518687</v>
+      </c>
+      <c r="D17">
+        <v>53.611817426979542</v>
+      </c>
+      <c r="E17">
+        <v>4528</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>53360.074326238268</v>
+      </c>
+      <c r="C18">
+        <v>17634.267536148891</v>
+      </c>
+      <c r="D18">
+        <v>20.914825439453121</v>
+      </c>
+      <c r="E18">
+        <v>7566</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>142432.9869418719</v>
+      </c>
+      <c r="C19">
+        <v>27942.80219278032</v>
+      </c>
+      <c r="D19">
+        <v>106.9618110656738</v>
+      </c>
+      <c r="E19">
+        <v>18493</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>22534.426690201821</v>
+      </c>
+      <c r="C20">
+        <v>13521.03359153675</v>
+      </c>
+      <c r="D20">
+        <v>13.00000619888306</v>
+      </c>
+      <c r="E20">
+        <v>6783</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>36019.599144551321</v>
+      </c>
+      <c r="C21">
+        <v>101899.9311060513</v>
+      </c>
+      <c r="D21">
+        <v>15</v>
+      </c>
+      <c r="E21">
+        <v>26888</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>44931.394216805042</v>
+      </c>
+      <c r="C22">
+        <v>15658.98141698869</v>
+      </c>
+      <c r="D22">
+        <v>43.694000244140618</v>
+      </c>
+      <c r="E22">
+        <v>9879</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>2065.2194960153552</v>
+      </c>
+      <c r="C23">
+        <v>3165.1494227013841</v>
+      </c>
+      <c r="D23">
+        <v>3.555999994277955</v>
+      </c>
+      <c r="E23">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>58307.285501919381</v>
+      </c>
+      <c r="C24">
+        <v>42435.882811048607</v>
+      </c>
+      <c r="D24">
+        <v>52</v>
+      </c>
+      <c r="E24">
+        <v>18401</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>6129.6016807130982</v>
+      </c>
+      <c r="C25">
+        <v>3664.1685254104809</v>
+      </c>
+      <c r="D25">
+        <v>47.136669907300757</v>
+      </c>
+      <c r="E25">
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26">
+        <v>81801.968693185336</v>
+      </c>
+      <c r="C26">
+        <v>35378.383010706508</v>
+      </c>
+      <c r="D26">
+        <v>61.018611907958977</v>
+      </c>
+      <c r="E26">
+        <v>16026</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27">
+        <v>68844.202533932723</v>
+      </c>
+      <c r="C27">
+        <v>40335.801494839157</v>
+      </c>
+      <c r="D27">
+        <v>38.881500244140618</v>
+      </c>
+      <c r="E27">
+        <v>18619</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>19580.99561413093</v>
+      </c>
+      <c r="C28">
+        <v>15701.678312169301</v>
+      </c>
+      <c r="D28">
+        <v>35</v>
+      </c>
+      <c r="E28">
+        <v>8249</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29">
+        <v>169890.51320796809</v>
+      </c>
+      <c r="C29">
+        <v>66414.046891629958</v>
+      </c>
+      <c r="D29">
+        <v>134.96919822692871</v>
+      </c>
+      <c r="E29">
+        <v>24136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30">
+        <v>59047.747089468918</v>
+      </c>
+      <c r="C30">
+        <v>14156.128298277659</v>
+      </c>
+      <c r="D30">
+        <v>21.496932983398441</v>
+      </c>
+      <c r="E30">
+        <v>7347</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31">
+        <v>357445.95730624709</v>
+      </c>
+      <c r="C31">
+        <v>44629.031865117176</v>
+      </c>
+      <c r="D31">
+        <v>87.12722110748291</v>
+      </c>
+      <c r="E31">
+        <v>17069</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32">
+        <v>33840.568813167083</v>
+      </c>
+      <c r="C32">
+        <v>11788.292434716859</v>
+      </c>
+      <c r="D32">
+        <v>10</v>
+      </c>
+      <c r="E32">
+        <v>4548</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33">
+        <v>1243998.1307313109</v>
+      </c>
+      <c r="C33">
+        <v>125356.8620921487</v>
+      </c>
+      <c r="D33">
+        <v>166.05999755859381</v>
+      </c>
+      <c r="E33">
+        <v>81053</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>297302.65980893082</v>
+      </c>
+      <c r="C34">
+        <v>41099.007819179933</v>
+      </c>
+      <c r="D34">
+        <v>115.76584625244141</v>
+      </c>
+      <c r="E34">
+        <v>29933</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35">
+        <v>119995.2882208134</v>
+      </c>
+      <c r="C35">
+        <v>44779.039457428531</v>
+      </c>
+      <c r="D35">
+        <v>185.88043212890619</v>
+      </c>
+      <c r="E35">
+        <v>21575</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36">
+        <v>46790.190569169717</v>
+      </c>
+      <c r="C36">
+        <v>10277.512151710391</v>
+      </c>
+      <c r="D36">
+        <v>120</v>
+      </c>
+      <c r="E36">
+        <v>6781</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37">
+        <v>11173.03485777296</v>
+      </c>
+      <c r="C37">
+        <v>7161.7369636316753</v>
+      </c>
+      <c r="D37">
+        <v>3.8000011444091801</v>
+      </c>
+      <c r="E37">
+        <v>2139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38">
+        <v>468170.01108463207</v>
+      </c>
+      <c r="C38">
+        <v>51083.140346867993</v>
+      </c>
+      <c r="D38">
+        <v>170</v>
+      </c>
+      <c r="E38">
+        <v>32170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new time estimation based on new slicer config
</commit_message>
<xml_diff>
--- a/time_estimation/time_estimation.xlsx
+++ b/time_estimation/time_estimation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d18ab4ce63646fc5/Documenten/TU Delft/Thesis/Code/time_estimation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_15C1348A5B00D05637F83111595ED87656CD9F4A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD522825-34A1-4FA9-B15F-D2D6CDE0B13F}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_2BD5F5835B40D45543782411595ED87656CD6A1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58C730BB-4BC0-4225-AA66-C848EF7C41A8}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="28800" windowHeight="15290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,90 +37,93 @@
     <t>Time [s]</t>
   </si>
   <si>
+    <t>3D_Printer_test_fixed_stl_3rd_gen</t>
+  </si>
+  <si>
+    <t>acoustic_plate</t>
+  </si>
+  <si>
+    <t>Another_dremel_bit_holder</t>
+  </si>
+  <si>
+    <t>bathroom_paper_roll_holder_with_shelf</t>
+  </si>
+  <si>
     <t>Beam_100x30mm</t>
   </si>
   <si>
     <t>Beam_30x100mm</t>
   </si>
   <si>
+    <t>Cap</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
     <t>Cube_50mm</t>
   </si>
   <si>
+    <t>Cute_axolotl_v5</t>
+  </si>
+  <si>
+    <t>Cylinder</t>
+  </si>
+  <si>
     <t>Cylinder_10x50mm</t>
   </si>
   <si>
     <t>Cylinder_50x50mm</t>
   </si>
   <si>
+    <t>Dancing_Happy_Dragon</t>
+  </si>
+  <si>
+    <t>Dewalt_Drill_Holder</t>
+  </si>
+  <si>
+    <t>dragon_statue</t>
+  </si>
+  <si>
+    <t>Flexi-Rex-improved</t>
+  </si>
+  <si>
+    <t>Flexy_PLA</t>
+  </si>
+  <si>
+    <t>full_flexi_possuml</t>
+  </si>
+  <si>
+    <t>FU_COIN_FINAL_12_31</t>
+  </si>
+  <si>
+    <t>HairTieBobbyPinBox</t>
+  </si>
+  <si>
+    <t>Low_poly_otter_3</t>
+  </si>
+  <si>
+    <t>Modern_Geometric_Planter</t>
+  </si>
+  <si>
+    <t>name_plate</t>
+  </si>
+  <si>
+    <t>Octopus_with_top_hat_for_some_reason</t>
+  </si>
+  <si>
+    <t>PCIE_Display_Stand4</t>
+  </si>
+  <si>
+    <t>Philips_OneBlade_Razor_Station</t>
+  </si>
+  <si>
     <t>Plate_10mm</t>
   </si>
   <si>
     <t>Pyramid_40mm</t>
   </si>
   <si>
-    <t>3D_Printer_test_fixed_stl_3rd_gen</t>
-  </si>
-  <si>
-    <t>acoustic_plat</t>
-  </si>
-  <si>
-    <t>Another_dremel_bit_holder</t>
-  </si>
-  <si>
-    <t>bathroom_paper_roll_holder_with_shelf</t>
-  </si>
-  <si>
-    <t>Cap</t>
-  </si>
-  <si>
-    <t>Cute_axolotl_v5</t>
-  </si>
-  <si>
-    <t>Cylinder</t>
-  </si>
-  <si>
-    <t>Dancing_Happy_Dragon</t>
-  </si>
-  <si>
-    <t>Dewalt_Drill_Holder</t>
-  </si>
-  <si>
-    <t>ragon_statu</t>
-  </si>
-  <si>
-    <t>Flexi-Rex-improv</t>
-  </si>
-  <si>
-    <t>Flexy_PLA</t>
-  </si>
-  <si>
-    <t>full_flexi_possuml</t>
-  </si>
-  <si>
-    <t>FU_COIN_FINAL_12_31</t>
-  </si>
-  <si>
-    <t>HairTieBobbyPinBox</t>
-  </si>
-  <si>
-    <t>Low_poly_otter_3</t>
-  </si>
-  <si>
-    <t>Modern_Geometric_Planter</t>
-  </si>
-  <si>
-    <t>name_plat</t>
-  </si>
-  <si>
-    <t>Octopus_with_top_hat_for_some_reason</t>
-  </si>
-  <si>
-    <t>PCIE_Display_Stand4</t>
-  </si>
-  <si>
-    <t>Philips_OneBlade_Razor_Station</t>
-  </si>
-  <si>
     <t>RubberDuck</t>
   </si>
   <si>
@@ -133,7 +136,7 @@
     <t>SM_Buddha_print</t>
   </si>
   <si>
-    <t>Speed_Squar</t>
+    <t>Speed_Square</t>
   </si>
   <si>
     <t>Swan</t>
@@ -143,9 +146,6 @@
   </si>
   <si>
     <t>VaseV846</t>
-  </si>
-  <si>
-    <t>case</t>
   </si>
 </sst>
 </file>
@@ -221,10 +221,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -514,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -542,16 +538,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>90000</v>
+        <v>48701.611744031121</v>
       </c>
       <c r="C2">
-        <v>13800</v>
+        <v>42737.72194506447</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>60.522235870361328</v>
       </c>
       <c r="E2">
-        <v>8999</v>
+        <v>19552</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -559,16 +555,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>90000</v>
+        <v>313750.00000000017</v>
       </c>
       <c r="C3">
-        <v>13800</v>
+        <v>74000</v>
       </c>
       <c r="D3">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E3">
-        <v>6817</v>
+        <v>62430</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -576,16 +572,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>125000</v>
+        <v>143591.84771055059</v>
       </c>
       <c r="C4">
-        <v>15000</v>
+        <v>50565.076410959482</v>
       </c>
       <c r="D4">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="E4">
-        <v>8616</v>
+        <v>40092</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -593,16 +589,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>3924.3010299656939</v>
+        <v>632926.45120755211</v>
       </c>
       <c r="C5">
-        <v>1727.4993534451301</v>
+        <v>103166.7185681635</v>
       </c>
       <c r="D5">
-        <v>50</v>
+        <v>185.93342590332031</v>
       </c>
       <c r="E5">
-        <v>1720</v>
+        <v>148381</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -610,16 +606,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>98152.154952251323</v>
+        <v>90000</v>
       </c>
       <c r="C6">
-        <v>11779.615498434559</v>
+        <v>13800</v>
       </c>
       <c r="D6">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E6">
-        <v>6638</v>
+        <v>20559</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -627,16 +623,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>399999.99999999988</v>
+        <v>90000</v>
       </c>
       <c r="C7">
-        <v>88000</v>
+        <v>13800</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E7">
-        <v>30346</v>
+        <v>18452</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -644,16 +640,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>18475.209554036319</v>
+        <v>5378.5681143174716</v>
       </c>
       <c r="C8">
-        <v>4800.0001221054636</v>
+        <v>2548.046221391171</v>
       </c>
       <c r="D8">
-        <v>34.641017913818359</v>
+        <v>12.50000035762787</v>
       </c>
       <c r="E8">
-        <v>2578</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -661,16 +657,16 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>48701.611744031121</v>
+        <v>12756.302435755561</v>
       </c>
       <c r="C9">
-        <v>42737.72194506447</v>
+        <v>14777.15722902477</v>
       </c>
       <c r="D9">
-        <v>60.522235870361328</v>
+        <v>21.79999923706055</v>
       </c>
       <c r="E9">
-        <v>16440</v>
+        <v>6165</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -678,16 +674,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>313750.00000000017</v>
+        <v>125000</v>
       </c>
       <c r="C10">
-        <v>74000</v>
+        <v>15000</v>
       </c>
       <c r="D10">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="E10">
-        <v>26275</v>
+        <v>25012</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -695,16 +691,16 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>143591.84771055059</v>
+        <v>545347.3514940599</v>
       </c>
       <c r="C11">
-        <v>50565.076410959482</v>
+        <v>64131.482762952903</v>
       </c>
       <c r="D11">
-        <v>15</v>
+        <v>76.063808441162109</v>
       </c>
       <c r="E11">
-        <v>23167</v>
+        <v>95169</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -712,16 +708,16 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>632926.45120755211</v>
+        <v>10004.086661324771</v>
       </c>
       <c r="C12">
-        <v>103166.7185681635</v>
+        <v>10260.452771781769</v>
       </c>
       <c r="D12">
-        <v>185.93342590332031</v>
+        <v>56.5</v>
       </c>
       <c r="E12">
-        <v>59451</v>
+        <v>5960</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -729,310 +725,310 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>5378.5681143174716</v>
+        <v>3924.3010299656939</v>
       </c>
       <c r="C13">
-        <v>2548.046221391171</v>
+        <v>1727.4993534451301</v>
       </c>
       <c r="D13">
-        <v>12.50000035762787</v>
+        <v>50</v>
       </c>
       <c r="E13">
-        <v>1285</v>
+        <v>3493</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="B14">
-        <v>12756.302435755561</v>
+        <v>98152.154952251323</v>
       </c>
       <c r="C14">
-        <v>14777.15722902477</v>
+        <v>11779.615498434559</v>
       </c>
       <c r="D14">
-        <v>21.79999923706055</v>
+        <v>50</v>
       </c>
       <c r="E14">
-        <v>4743</v>
+        <v>19236</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15">
-        <v>545347.3514940599</v>
+        <v>11907.500194774781</v>
       </c>
       <c r="C15">
-        <v>64131.482762952903</v>
+        <v>8387.9595668518687</v>
       </c>
       <c r="D15">
-        <v>76.063808441162109</v>
+        <v>53.611817426979542</v>
       </c>
       <c r="E15">
-        <v>29663</v>
+        <v>6038</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16">
-        <v>10004.086661324771</v>
+        <v>53360.074326238268</v>
       </c>
       <c r="C16">
-        <v>10260.452771781769</v>
+        <v>17634.267536148891</v>
       </c>
       <c r="D16">
-        <v>56.5</v>
+        <v>20.914825439453121</v>
       </c>
       <c r="E16">
-        <v>4778</v>
+        <v>13314</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17">
-        <v>11907.500194774781</v>
+        <v>142432.9869418719</v>
       </c>
       <c r="C17">
-        <v>8387.9595668518687</v>
+        <v>27942.80219278032</v>
       </c>
       <c r="D17">
-        <v>53.611817426979542</v>
+        <v>106.9618110656738</v>
       </c>
       <c r="E17">
-        <v>4528</v>
+        <v>40828</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B18">
-        <v>53360.074326238268</v>
+        <v>22534.426690201821</v>
       </c>
       <c r="C18">
-        <v>17634.267536148891</v>
+        <v>13521.03359153675</v>
       </c>
       <c r="D18">
-        <v>20.914825439453121</v>
+        <v>13.00000619888306</v>
       </c>
       <c r="E18">
-        <v>7566</v>
+        <v>9471</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B19">
-        <v>142432.9869418719</v>
+        <v>36019.599144551321</v>
       </c>
       <c r="C19">
-        <v>27942.80219278032</v>
+        <v>101899.9311060513</v>
       </c>
       <c r="D19">
-        <v>106.9618110656738</v>
+        <v>15</v>
       </c>
       <c r="E19">
-        <v>18493</v>
+        <v>26859</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20">
-        <v>22534.426690201821</v>
+        <v>44931.394216805042</v>
       </c>
       <c r="C20">
-        <v>13521.03359153675</v>
+        <v>15658.98141698869</v>
       </c>
       <c r="D20">
-        <v>13.00000619888306</v>
+        <v>43.694000244140618</v>
       </c>
       <c r="E20">
-        <v>6783</v>
+        <v>16786</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21">
-        <v>36019.599144551321</v>
+        <v>2065.2194960153552</v>
       </c>
       <c r="C21">
-        <v>101899.9311060513</v>
+        <v>3165.1494227013841</v>
       </c>
       <c r="D21">
-        <v>15</v>
+        <v>3.555999994277955</v>
       </c>
       <c r="E21">
-        <v>26888</v>
+        <v>944</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22">
-        <v>44931.394216805042</v>
+        <v>58307.285501919381</v>
       </c>
       <c r="C22">
-        <v>15658.98141698869</v>
+        <v>42435.882811048607</v>
       </c>
       <c r="D22">
-        <v>43.694000244140618</v>
+        <v>52</v>
       </c>
       <c r="E22">
-        <v>9879</v>
+        <v>26629</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23">
-        <v>2065.2194960153552</v>
+        <v>6129.6016807130982</v>
       </c>
       <c r="C23">
-        <v>3165.1494227013841</v>
+        <v>3664.1685254104809</v>
       </c>
       <c r="D23">
-        <v>3.555999994277955</v>
+        <v>47.136669907300757</v>
       </c>
       <c r="E23">
-        <v>824</v>
+        <v>3901</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B24">
-        <v>58307.285501919381</v>
+        <v>81801.968693185336</v>
       </c>
       <c r="C24">
-        <v>42435.882811048607</v>
+        <v>35378.383010706508</v>
       </c>
       <c r="D24">
-        <v>52</v>
+        <v>61.018611907958977</v>
       </c>
       <c r="E24">
-        <v>18401</v>
+        <v>29981</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B25">
-        <v>6129.6016807130982</v>
+        <v>68844.202533932723</v>
       </c>
       <c r="C25">
-        <v>3664.1685254104809</v>
+        <v>40335.801494839157</v>
       </c>
       <c r="D25">
-        <v>47.136669907300757</v>
+        <v>38.881500244140618</v>
       </c>
       <c r="E25">
-        <v>2640</v>
+        <v>32891</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B26">
-        <v>81801.968693185336</v>
+        <v>19580.99561413093</v>
       </c>
       <c r="C26">
-        <v>35378.383010706508</v>
+        <v>15701.678312169301</v>
       </c>
       <c r="D26">
-        <v>61.018611907958977</v>
+        <v>35</v>
       </c>
       <c r="E26">
-        <v>16026</v>
+        <v>11148</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27">
-        <v>68844.202533932723</v>
+        <v>169890.51320796809</v>
       </c>
       <c r="C27">
-        <v>40335.801494839157</v>
+        <v>66414.046891629958</v>
       </c>
       <c r="D27">
-        <v>38.881500244140618</v>
+        <v>134.96919822692871</v>
       </c>
       <c r="E27">
-        <v>18619</v>
+        <v>47868</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B28">
-        <v>19580.99561413093</v>
+        <v>59047.747089468918</v>
       </c>
       <c r="C28">
-        <v>15701.678312169301</v>
+        <v>14156.128298277659</v>
       </c>
       <c r="D28">
-        <v>35</v>
+        <v>21.496932983398441</v>
       </c>
       <c r="E28">
-        <v>8249</v>
+        <v>15679</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B29">
-        <v>169890.51320796809</v>
+        <v>399999.99999999988</v>
       </c>
       <c r="C29">
-        <v>66414.046891629958</v>
+        <v>88000</v>
       </c>
       <c r="D29">
-        <v>134.96919822692871</v>
+        <v>10</v>
       </c>
       <c r="E29">
-        <v>24136</v>
+        <v>71282</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B30">
-        <v>59047.747089468918</v>
+        <v>18475.209554036319</v>
       </c>
       <c r="C30">
-        <v>14156.128298277659</v>
+        <v>4800.0001221054636</v>
       </c>
       <c r="D30">
-        <v>21.496932983398441</v>
+        <v>34.641017913818359</v>
       </c>
       <c r="E30">
-        <v>7347</v>
+        <v>4850</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31">
         <v>357445.95730624709</v>
@@ -1044,12 +1040,12 @@
         <v>87.12722110748291</v>
       </c>
       <c r="E31">
-        <v>17069</v>
+        <v>52696</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B32">
         <v>33840.568813167083</v>
@@ -1061,12 +1057,12 @@
         <v>10</v>
       </c>
       <c r="E32">
-        <v>4548</v>
+        <v>8233</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B33">
         <v>1243998.1307313109</v>
@@ -1078,12 +1074,12 @@
         <v>166.05999755859381</v>
       </c>
       <c r="E33">
-        <v>81053</v>
+        <v>252230</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B34">
         <v>297302.65980893082</v>
@@ -1095,12 +1091,12 @@
         <v>115.76584625244141</v>
       </c>
       <c r="E34">
-        <v>29933</v>
+        <v>72176</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35">
         <v>119995.2882208134</v>
@@ -1112,12 +1108,12 @@
         <v>185.88043212890619</v>
       </c>
       <c r="E35">
-        <v>21575</v>
+        <v>36639</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36">
         <v>46790.190569169717</v>
@@ -1129,12 +1125,12 @@
         <v>120</v>
       </c>
       <c r="E36">
-        <v>6781</v>
+        <v>14371</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B37">
         <v>11173.03485777296</v>
@@ -1146,12 +1142,12 @@
         <v>3.8000011444091801</v>
       </c>
       <c r="E37">
-        <v>2139</v>
+        <v>2708</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B38">
         <v>468170.01108463207</v>
@@ -1163,7 +1159,7 @@
         <v>170</v>
       </c>
       <c r="E38">
-        <v>32170</v>
+        <v>102112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>